<commit_message>
OO Tic Tac Toe Bonus - AI Defense
</commit_message>
<xml_diff>
--- a/lesson_5/Tic_Tac_Toe_CRC.xlsx
+++ b/lesson_5/Tic_Tac_Toe_CRC.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41D1521-1639-884C-B9EE-E3562A3D2A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E4BDD4-9121-6544-9401-67F5B741E830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
+    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="2" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Game" sheetId="1" r:id="rId1"/>
     <sheet name="Scored Game" sheetId="2" r:id="rId2"/>
+    <sheet name="AI Defense" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="133">
   <si>
     <t>Board</t>
   </si>
@@ -260,9 +261,6 @@
     <t>Can determine if human move</t>
   </si>
   <si>
-    <t>human_move?</t>
-  </si>
-  <si>
     <t>Can make human move</t>
   </si>
   <si>
@@ -369,6 +367,75 @@
   </si>
   <si>
     <t>If yes, reset scores and game</t>
+  </si>
+  <si>
+    <t>@board, @human, @computer, @scores, @current_player</t>
+  </si>
+  <si>
+    <t>SCORE_THRESHOLD</t>
+  </si>
+  <si>
+    <t>Has a score array</t>
+  </si>
+  <si>
+    <t>@scores</t>
+  </si>
+  <si>
+    <t>human_turn?</t>
+  </si>
+  <si>
+    <t>Can increment player scores</t>
+  </si>
+  <si>
+    <t>increment_scores</t>
+  </si>
+  <si>
+    <t>can update score for a player</t>
+  </si>
+  <si>
+    <t>update_score</t>
+  </si>
+  <si>
+    <t>display_game_result</t>
+  </si>
+  <si>
+    <t>Can display match result</t>
+  </si>
+  <si>
+    <t>display_match_result</t>
+  </si>
+  <si>
+    <t>Can display player scores</t>
+  </si>
+  <si>
+    <t>display_match_scores</t>
+  </si>
+  <si>
+    <t>reset_game</t>
+  </si>
+  <si>
+    <t>Can determine match winner(s)</t>
+  </si>
+  <si>
+    <t>Can determine if player(s) won match</t>
+  </si>
+  <si>
+    <t>player_won_match?</t>
+  </si>
+  <si>
+    <t>match_winners</t>
+  </si>
+  <si>
+    <t>Can reset match</t>
+  </si>
+  <si>
+    <t>reset_match</t>
+  </si>
+  <si>
+    <t>Tic Tac Toe Class Responsibility Collaborator Cards - AI Defense</t>
+  </si>
+  <si>
+    <t>Parent method</t>
   </si>
 </sst>
 </file>
@@ -1615,14 +1682,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>918482</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>170089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1927678</xdr:colOff>
+      <xdr:colOff>1890889</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
+      <xdr:rowOff>122297</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1637,8 +1704,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7014482" y="6215289"/>
-          <a:ext cx="9264196" cy="2536825"/>
+          <a:off x="8359741" y="7319719"/>
+          <a:ext cx="9213296" cy="1513837"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1668,14 +1735,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>918482</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>102053</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1916339</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:colOff>1900296</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>102053</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1689,9 +1756,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="7014482" y="7036253"/>
-          <a:ext cx="9252857" cy="1704522"/>
+        <a:xfrm flipH="1">
+          <a:off x="8359741" y="8833556"/>
+          <a:ext cx="9222703" cy="873460"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1720,15 +1787,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>850446</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
+      <xdr:colOff>903111</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1916339</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>103481</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1742,9 +1809,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="6946446" y="7425871"/>
-          <a:ext cx="9320893" cy="1326243"/>
+        <a:xfrm flipH="1">
+          <a:off x="8344370" y="8833556"/>
+          <a:ext cx="9228667" cy="1053629"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1773,15 +1840,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>884464</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
+      <xdr:colOff>799630</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>159926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
+      <xdr:colOff>1900296</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
+      <xdr:rowOff>112889</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1796,8 +1863,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6980464" y="8396514"/>
-          <a:ext cx="9275536" cy="355600"/>
+          <a:off x="8240889" y="8156222"/>
+          <a:ext cx="9341555" cy="667926"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1827,13 +1894,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>703036</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>136071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1950357</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1880,13 +1947,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>855436</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>124733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1893660</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>107044</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1933,13 +2000,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1564822</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>124732</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1927678</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1986,13 +2053,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>884465</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>90715</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1961696</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>147411</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2039,13 +2106,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1678215</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1961696</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>22678</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2091,15 +2158,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>832757</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:colOff>1185333</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>79375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1961696</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>129722</xdr:rowOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2114,8 +2181,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4960257" y="5057775"/>
-          <a:ext cx="5256439" cy="2183947"/>
+          <a:off x="6566370" y="5441597"/>
+          <a:ext cx="4896807" cy="3043884"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2144,15 +2211,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1626507</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:colOff>1749778</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>147411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1950357</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>4989</xdr:rowOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>65852</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2167,8 +2234,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5754007" y="4770211"/>
-          <a:ext cx="4451350" cy="2524578"/>
+          <a:off x="7130815" y="5152152"/>
+          <a:ext cx="4321023" cy="3314515"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2197,15 +2264,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>832757</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:colOff>1345259</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>147411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1950357</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>147408</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>122296</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2220,8 +2287,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4960257" y="5659211"/>
-          <a:ext cx="5245100" cy="2616197"/>
+          <a:off x="6820370" y="6045855"/>
+          <a:ext cx="4725543" cy="1762293"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2250,15 +2317,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>725715</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>743185</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>113392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1961696</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94074</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2273,8 +2340,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4853215" y="5802992"/>
-          <a:ext cx="5363481" cy="2937783"/>
+          <a:off x="6218296" y="6190577"/>
+          <a:ext cx="5338956" cy="1946830"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2304,13 +2371,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>771071</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>113393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1927678</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>113392</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2357,13 +2424,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1065893</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>113393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1916339</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>113392</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2410,13 +2477,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>907143</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>118382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1909989</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>79375</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2463,13 +2530,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>827768</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>113393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1950357</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2516,14 +2583,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>669018</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>113393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1927678</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>102053</xdr:rowOff>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2538,8 +2605,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6765018" y="3847193"/>
-          <a:ext cx="9513660" cy="5449660"/>
+          <a:off x="8110277" y="4045689"/>
+          <a:ext cx="9462760" cy="5465200"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2569,14 +2636,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>669018</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>113393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1939017</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>113393</xdr:rowOff>
+      <xdr:colOff>1872074</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>75259</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2591,8 +2658,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6765018" y="4024993"/>
-          <a:ext cx="9524999" cy="5283200"/>
+          <a:off x="8110277" y="4224430"/>
+          <a:ext cx="9443945" cy="5277051"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2622,13 +2689,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>680357</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>124733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1927678</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>102054</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2675,13 +2742,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>113393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1893660</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>124732</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2699,6 +2766,1124 @@
         <a:xfrm flipH="1">
           <a:off x="12985750" y="3135993"/>
           <a:ext cx="3258910" cy="2678339"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>918482</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>170089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ADC63AD-2497-4545-9CEA-5ED86C42B9F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8360682" y="7282089"/>
+          <a:ext cx="9227407" cy="1501608"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>918482</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1900296</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>102053</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35A16671-3350-7E49-988E-6A68766FA6F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8360682" y="8783697"/>
+          <a:ext cx="9236814" cy="868756"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>903111</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>103481</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51367888-E7DE-1546-BEE3-D125E4CA719A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8345311" y="8783697"/>
+          <a:ext cx="9242778" cy="1047984"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>799630</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>159926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1900296</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>112889</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{656F6623-002D-B04E-A677-67E2DEBAE73E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8241830" y="8110126"/>
+          <a:ext cx="9355666" cy="664163"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>703036</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACA96B37-2219-9C4F-A404-EE5D580AE017}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6176736" y="5292271"/>
+          <a:ext cx="5374821" cy="1955801"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>855436</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>124733</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1893660</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>107044</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D04DB14A-54D0-274A-A4BD-E09C18F39B3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6329136" y="5814333"/>
+          <a:ext cx="5165724" cy="1582511"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1564822</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>124732</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1927678</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE7574DE-AA1E-E34F-9D7B-6781E171987E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7038522" y="5636532"/>
+          <a:ext cx="4490356" cy="1831068"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>884465</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>90715</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1961696</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>147411</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AC7A3DC-C84E-894E-B760-2F94237A1748}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6358165" y="5424715"/>
+          <a:ext cx="5204731" cy="4095296"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1678215</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1961696</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>22678</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C524BEA2-59DB-534F-8C11-DF39B3EC135C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7151915" y="5114472"/>
+          <a:ext cx="4410981" cy="4458606"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1185333</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1961696</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FFB4A34-21C9-3A41-95D9-2C01E5968CDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6659033" y="5413375"/>
+          <a:ext cx="4903863" cy="4399491"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1749778</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>147411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>65852</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06AD82AB-0438-0D4A-B589-4495D7038891}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7223478" y="5125811"/>
+          <a:ext cx="4328079" cy="4668241"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1345259</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>147411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>122296</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FED7527-9D85-8D46-993F-BDE760C6B240}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6818959" y="6014811"/>
+          <a:ext cx="4732598" cy="2057685"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>743185</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>113392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1961696</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94074</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B76A354-0953-5E48-9B4F-F5F6B22B809A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6216885" y="6158592"/>
+          <a:ext cx="5346011" cy="2241282"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>771071</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1927678</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113392</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3163392-F242-A74B-8B4D-BF953A99D779}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14309271" y="5091793"/>
+          <a:ext cx="3315607" cy="177799"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1065893</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1916339</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>113392</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30664133-5284-DD40-9786-2B7A1BF060D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14604093" y="5269593"/>
+          <a:ext cx="3009446" cy="177799"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>907143</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1909989</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB163437-B6F0-1742-99D3-11D90874AF7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14445343" y="5452382"/>
+          <a:ext cx="3161846" cy="2094593"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>827768</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3902D7F8-3E70-AC44-8386-ACFB7C1B4FB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14365968" y="2780393"/>
+          <a:ext cx="3281589" cy="3223078"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>669018</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79919739-378D-0547-98CB-FC4DABA0548D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8111218" y="4024993"/>
+          <a:ext cx="9476871" cy="5432274"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>669018</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1872074</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>75259</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01CBE6F5-1DA8-D740-B914-E123C545F084}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8111218" y="4202793"/>
+          <a:ext cx="9458056" cy="5245066"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>680357</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>124733</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1927678</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>102054</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14A5E8FD-4685-2E4B-937D-AE81233A9C7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6154057" y="3325133"/>
+          <a:ext cx="5374821" cy="510721"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>793750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1893660</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>124732</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DDF2F3C-6981-4147-8D90-FC4040004689}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14331950" y="3313793"/>
+          <a:ext cx="3258910" cy="2856139"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3026,9 +4211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B44A927-A882-3743-B3D8-A9052DE973A6}">
   <dimension ref="B1:M60"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3045,7 +4228,7 @@
     <row r="1" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:13" ht="26" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.2"/>
@@ -3082,31 +4265,31 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="3"/>
       <c r="G6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -3146,27 +4329,27 @@
     <row r="11" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>36</v>
@@ -3174,16 +4357,16 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>36</v>
@@ -3192,22 +4375,22 @@
     <row r="15" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
         <v>99</v>
       </c>
-      <c r="C16" t="s">
-        <v>100</v>
-      </c>
       <c r="G16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" t="s">
         <v>99</v>
       </c>
-      <c r="H16" t="s">
-        <v>100</v>
-      </c>
       <c r="K16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" t="s">
         <v>99</v>
-      </c>
-      <c r="L16" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2"/>
@@ -3234,13 +4417,13 @@
         <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>36</v>
@@ -3353,7 +4536,7 @@
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G28" t="s">
         <v>56</v>
@@ -3390,7 +4573,7 @@
         <v>51</v>
       </c>
       <c r="I30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
@@ -3422,7 +4605,7 @@
         <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
@@ -3438,7 +4621,7 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G35" t="s">
         <v>46</v>
@@ -3463,43 +4646,43 @@
         <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
         <v>91</v>
-      </c>
-      <c r="C39" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" t="s">
         <v>76</v>
       </c>
-      <c r="C40" t="s">
-        <v>79</v>
-      </c>
-      <c r="D40" t="s">
-        <v>77</v>
-      </c>
       <c r="E40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="2:12" ht="19" x14ac:dyDescent="0.25">
@@ -3520,10 +4703,10 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="K43" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="L43" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
@@ -3540,10 +4723,10 @@
         <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -3553,7 +4736,7 @@
         <v>33</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
@@ -3564,10 +4747,10 @@
         <v>49</v>
       </c>
       <c r="D47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>36</v>
@@ -3575,23 +4758,23 @@
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
         <v>82</v>
       </c>
-      <c r="C48" t="s">
-        <v>83</v>
-      </c>
       <c r="K48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="11:12" x14ac:dyDescent="0.2"/>
     <row r="50" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L50" t="s">
         <v>99</v>
-      </c>
-      <c r="L50" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="51" spans="11:12" x14ac:dyDescent="0.2">
@@ -3638,15 +4821,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D4ED49-275E-7E4A-BA8A-0F7580125B37}">
-  <dimension ref="B1:N60"/>
+  <dimension ref="B1:N90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="135" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="19.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="31" customWidth="1"/>
+    <col min="3" max="3" width="32.3984375" customWidth="1"/>
+    <col min="4" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
     <col min="8" max="10" width="31" customWidth="1"/>
     <col min="11" max="11" width="3" customWidth="1"/>
@@ -3655,17 +4839,18 @@
     <col min="15" max="16384" width="11" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:14" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="3:14" ht="26" x14ac:dyDescent="0.3">
-      <c r="C2" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="3:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="10" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:14" ht="26" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -3682,7 +4867,7 @@
       <c r="M4" s="10"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="3:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="6"/>
       <c r="G5" s="3"/>
       <c r="H5" s="6"/>
@@ -3693,37 +4878,40 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="C6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="3"/>
       <c r="H6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
@@ -3735,7 +4923,7 @@
       </c>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>9</v>
       </c>
@@ -3746,136 +4934,130 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="1" t="s">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H13" t="s">
-        <v>93</v>
-      </c>
-      <c r="L13" t="s">
-        <v>93</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="H13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C16" s="2" t="s">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="L15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
         <v>99</v>
       </c>
-      <c r="D16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="H17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
         <v>99</v>
       </c>
-      <c r="I16" t="s">
-        <v>100</v>
-      </c>
-      <c r="L16" s="2" t="s">
+      <c r="L17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" t="s">
         <v>99</v>
       </c>
-      <c r="M16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C18" s="2" t="s">
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" t="s">
-        <v>96</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L19" t="s">
-        <v>95</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="M19" s="2"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>67</v>
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" t="s">
+        <v>94</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
         <v>67</v>
@@ -3883,116 +5065,101 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D23" s="1"/>
-    </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="L26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I27" t="s">
         <v>61</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L27" t="s">
         <v>38</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="H26" t="s">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
         <v>58</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I28" t="s">
         <v>59</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J28" t="s">
         <v>64</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L28" t="s">
         <v>40</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C27" s="2" t="s">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H29" t="s">
         <v>54</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I29" t="s">
         <v>55</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J29" t="s">
         <v>62</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L29" t="s">
         <v>41</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M29" s="4" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" t="s">
-        <v>56</v>
-      </c>
-      <c r="I28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
@@ -4000,19 +5167,16 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="H30" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I30" t="s">
-        <v>51</v>
-      </c>
-      <c r="J30" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
@@ -4020,135 +5184,156 @@
         <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="I31" t="s">
-        <v>49</v>
-      </c>
-      <c r="J31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" t="s">
-        <v>86</v>
+        <v>121</v>
+      </c>
+      <c r="H33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J33" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="H34" s="2" t="s">
-        <v>19</v>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" t="s">
-        <v>90</v>
-      </c>
-      <c r="H35" t="s">
-        <v>46</v>
-      </c>
-      <c r="I35" t="s">
-        <v>47</v>
-      </c>
-      <c r="J35" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" t="s">
-        <v>86</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>123</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" t="s">
-        <v>77</v>
-      </c>
-      <c r="F40" t="s">
-        <v>86</v>
+        <v>29</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="2:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J41" t="s">
+        <v>63</v>
+      </c>
       <c r="L41" s="10" t="s">
         <v>2</v>
       </c>
@@ -4156,26 +5341,50 @@
     </row>
     <row r="42" spans="2:13" ht="19" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="D42" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="L42" s="6"/>
       <c r="M42" s="3"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" t="s">
+        <v>85</v>
+      </c>
       <c r="L43" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M43" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M43" s="5" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" t="s">
+        <v>127</v>
+      </c>
       <c r="L44" s="2" t="s">
         <v>22</v>
       </c>
@@ -4186,49 +5395,34 @@
         <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F45" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" t="s">
-        <v>103</v>
-      </c>
       <c r="L46" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="L47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>36</v>
@@ -4236,89 +5430,995 @@
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
-      </c>
-      <c r="L48" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="L50" s="2" t="s">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
+        <v>93</v>
+      </c>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M51" t="s">
         <v>99</v>
       </c>
-      <c r="M50" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="L51" s="2"/>
-    </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C52" s="2" t="s">
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" t="s">
+        <v>76</v>
+      </c>
+      <c r="F52" t="s">
+        <v>85</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" t="s">
+        <v>76</v>
+      </c>
+      <c r="F53" t="s">
+        <v>85</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C61" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C62" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="L52" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M52" s="2"/>
-    </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L53" t="s">
-        <v>35</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="54" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C64" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C55" s="2" t="s">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C56" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C57" s="2" t="s">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C58" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M58" s="2"/>
-    </row>
-    <row r="59" spans="3:13" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="81" x14ac:dyDescent="0.2"/>
+    <row r="82" x14ac:dyDescent="0.2"/>
+    <row r="83" x14ac:dyDescent="0.2"/>
+    <row r="84" x14ac:dyDescent="0.2"/>
+    <row r="85" x14ac:dyDescent="0.2"/>
+    <row r="86" x14ac:dyDescent="0.2"/>
+    <row r="87" x14ac:dyDescent="0.2"/>
+    <row r="88" x14ac:dyDescent="0.2"/>
+    <row r="89" x14ac:dyDescent="0.2"/>
+    <row r="90" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C4:F4"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="L41:M41"/>
+    <mergeCell ref="B4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624FF2EF-F1A6-254C-9967-68AF7C1C66F8}">
+  <dimension ref="B1:N90"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.3984375" customWidth="1"/>
+    <col min="4" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="8" max="10" width="31" customWidth="1"/>
+    <col min="11" max="11" width="3" customWidth="1"/>
+    <col min="12" max="13" width="31" customWidth="1"/>
+    <col min="14" max="14" width="3" customWidth="1"/>
+    <col min="15" max="16384" width="11" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:14" ht="26" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="L15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" t="s">
+        <v>94</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" t="s">
+        <v>41</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J41" t="s">
+        <v>63</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="2:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" t="s">
+        <v>116</v>
+      </c>
+      <c r="L42" s="6"/>
+      <c r="M42" s="3"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" t="s">
+        <v>85</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" t="s">
+        <v>127</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" t="s">
+        <v>83</v>
+      </c>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L46" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" t="s">
+        <v>70</v>
+      </c>
+      <c r="L47" t="s">
+        <v>92</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
+        <v>93</v>
+      </c>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" t="s">
+        <v>76</v>
+      </c>
+      <c r="F52" t="s">
+        <v>85</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" t="s">
+        <v>76</v>
+      </c>
+      <c r="F53" t="s">
+        <v>85</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C61" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C62" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C64" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="81" x14ac:dyDescent="0.2"/>
+    <row r="82" x14ac:dyDescent="0.2"/>
+    <row r="83" x14ac:dyDescent="0.2"/>
+    <row r="84" x14ac:dyDescent="0.2"/>
+    <row r="85" x14ac:dyDescent="0.2"/>
+    <row r="86" x14ac:dyDescent="0.2"/>
+    <row r="87" x14ac:dyDescent="0.2"/>
+    <row r="88" x14ac:dyDescent="0.2"/>
+    <row r="89" x14ac:dyDescent="0.2"/>
+    <row r="90" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
OO Tic Tac Toe Bonus - AI Offense
</commit_message>
<xml_diff>
--- a/lesson_5/Tic_Tac_Toe_CRC.xlsx
+++ b/lesson_5/Tic_Tac_Toe_CRC.xlsx
@@ -2,20 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E4BDD4-9121-6544-9401-67F5B741E830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CB30E3-FB2B-A34B-A0A1-5DE189E7DF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="2" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
+    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Game" sheetId="1" r:id="rId1"/>
     <sheet name="Scored Game" sheetId="2" r:id="rId2"/>
     <sheet name="AI Defense" sheetId="3" r:id="rId3"/>
+    <sheet name="AI Offense" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="144">
   <si>
     <t>Board</t>
   </si>
@@ -436,6 +437,39 @@
   </si>
   <si>
     <t>Parent method</t>
+  </si>
+  <si>
+    <t>Can determine if square(s) threatened</t>
+  </si>
+  <si>
+    <t>squares_threatened</t>
+  </si>
+  <si>
+    <t>Has two player markers and one empty</t>
+  </si>
+  <si>
+    <t>two_taken_one_empty?</t>
+  </si>
+  <si>
+    <t>empty_square</t>
+  </si>
+  <si>
+    <t>Can find first empty square</t>
+  </si>
+  <si>
+    <t>Board.squares_threatened</t>
+  </si>
+  <si>
+    <t>Tic Tac Toe Class Responsibility Collaborator Cards - AI Offense</t>
+  </si>
+  <si>
+    <t>Board.third_square_available</t>
+  </si>
+  <si>
+    <t>third_square_available</t>
+  </si>
+  <si>
+    <t>Can determine if one empty in line</t>
   </si>
 </sst>
 </file>
@@ -3013,11 +3047,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>703036</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
+      <xdr:rowOff>111760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:colOff>2113280</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
@@ -3034,8 +3068,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6176736" y="5292271"/>
-          <a:ext cx="5374821" cy="1955801"/>
+          <a:off x="6189436" y="5405120"/>
+          <a:ext cx="5545364" cy="2035992"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3066,11 +3100,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>855436</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>124733</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1893660</xdr:colOff>
+      <xdr:colOff>2082800</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>107044</xdr:rowOff>
     </xdr:to>
@@ -3087,8 +3121,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6329136" y="5814333"/>
-          <a:ext cx="5165724" cy="1582511"/>
+          <a:off x="6341836" y="5943600"/>
+          <a:ext cx="5362484" cy="1651364"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3119,11 +3153,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1564822</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>124732</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1927678</xdr:colOff>
+      <xdr:colOff>2113280</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -3140,8 +3174,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7038522" y="5636532"/>
-          <a:ext cx="4490356" cy="1831068"/>
+          <a:off x="7051222" y="5781040"/>
+          <a:ext cx="4683578" cy="1889760"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3172,11 +3206,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>884465</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>90715</xdr:rowOff>
+      <xdr:rowOff>142240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1961696</xdr:colOff>
+      <xdr:colOff>2092960</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>147411</xdr:rowOff>
     </xdr:to>
@@ -3193,8 +3227,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6358165" y="5424715"/>
-          <a:ext cx="5204731" cy="4095296"/>
+          <a:off x="6370865" y="5618480"/>
+          <a:ext cx="5343615" cy="4150451"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3225,11 +3259,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1678215</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>136072</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1961696</xdr:colOff>
+      <xdr:colOff>2092960</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>22678</xdr:rowOff>
     </xdr:to>
@@ -3246,8 +3280,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7151915" y="5114472"/>
-          <a:ext cx="4410981" cy="4458606"/>
+          <a:off x="7164615" y="5201920"/>
+          <a:ext cx="4549865" cy="4625158"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3278,11 +3312,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1185333</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1961696</xdr:colOff>
+      <xdr:colOff>2103120</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>84666</xdr:rowOff>
     </xdr:to>
@@ -3299,8 +3333,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6659033" y="5413375"/>
-          <a:ext cx="4903863" cy="4399491"/>
+          <a:off x="6671733" y="5598160"/>
+          <a:ext cx="5052907" cy="4473786"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3331,11 +3365,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1749778</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>147411</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:colOff>2092960</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>65852</xdr:rowOff>
     </xdr:to>
@@ -3352,8 +3386,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7223478" y="5125811"/>
-          <a:ext cx="4328079" cy="4668241"/>
+          <a:off x="7236178" y="5212080"/>
+          <a:ext cx="4478302" cy="4841052"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3384,11 +3418,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1345259</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>147411</xdr:rowOff>
+      <xdr:rowOff>132080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:colOff>2072640</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>122296</xdr:rowOff>
     </xdr:to>
@@ -3405,8 +3439,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6818959" y="6014811"/>
-          <a:ext cx="4732598" cy="2057685"/>
+          <a:off x="6831659" y="6156960"/>
+          <a:ext cx="4862501" cy="2123816"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3437,11 +3471,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>743185</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>113392</xdr:rowOff>
+      <xdr:rowOff>111760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1961696</xdr:colOff>
+      <xdr:colOff>2103120</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>94074</xdr:rowOff>
     </xdr:to>
@@ -3458,8 +3492,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6216885" y="6158592"/>
-          <a:ext cx="5346011" cy="2241282"/>
+          <a:off x="6229585" y="6319520"/>
+          <a:ext cx="5495055" cy="2298794"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3808,11 +3842,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>680357</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>124733</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1927678</xdr:colOff>
+      <xdr:colOff>2092960</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>102054</xdr:rowOff>
     </xdr:to>
@@ -3829,8 +3863,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6154057" y="3325133"/>
-          <a:ext cx="5374821" cy="510721"/>
+          <a:off x="6166757" y="3373120"/>
+          <a:ext cx="5547723" cy="559254"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3901,6 +3935,1230 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1574800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E81910-A552-B540-B594-8CE8F0113C8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7061200" y="6482080"/>
+          <a:ext cx="4663440" cy="3810000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>918482</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>170089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AE39E60-4683-BD4A-9A6F-85E75050ECC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8360682" y="7282089"/>
+          <a:ext cx="9405207" cy="1501608"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>918482</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1900296</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>102053</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{116AB56A-A175-5D4E-A4CA-7EA3E7E0EA69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8360682" y="8783697"/>
+          <a:ext cx="9414614" cy="868756"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>903111</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>103481</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F744641-8D30-9944-B3D0-792882567A04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8345311" y="8783697"/>
+          <a:ext cx="9420578" cy="1047984"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>799630</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>159926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1900296</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>112889</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0964A8F0-F4C5-554C-B1DB-30321B6B87FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8241830" y="8110126"/>
+          <a:ext cx="9533466" cy="664163"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>703036</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2113280</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59069BB8-64B9-854C-8D15-A5B2C1C35BB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6176736" y="5267960"/>
+          <a:ext cx="5537744" cy="1980112"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>855436</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2082800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>107044</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BEC0E5C-B5B2-1943-B7A6-A68B4DBEE5FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6329136" y="5791200"/>
+          <a:ext cx="5354864" cy="1605644"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1564822</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2113280</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCF3FFAD-0BCD-D649-914D-ED5EB2F7A08C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7038522" y="5633720"/>
+          <a:ext cx="4675958" cy="1833880"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>884465</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2092960</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>147411</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6464065F-5495-F14F-90A6-7B3C34F97F7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6358165" y="5476240"/>
+          <a:ext cx="5335995" cy="4043771"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1678215</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2092960</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>22678</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{244F5557-F738-934D-88AF-C0EBDF56A3A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7151915" y="5069840"/>
+          <a:ext cx="4542245" cy="4503238"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1185333</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37F691A8-305C-264C-AC67-246DD4C63280}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6659033" y="5455920"/>
+          <a:ext cx="5045287" cy="4356946"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1749778</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2092960</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>65852</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF40A96F-3B11-524A-814F-BC3D9E112A16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7223478" y="5080000"/>
+          <a:ext cx="4470682" cy="4714052"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1345259</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2072640</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>122296</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEBDD878-E3A1-364E-85BD-F6E4EC90AC04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6818959" y="5999480"/>
+          <a:ext cx="4854881" cy="2073016"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>743185</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94074</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B8748DF-826D-9543-B3E2-09D0A25AA799}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6216885" y="6156960"/>
+          <a:ext cx="5487435" cy="2242914"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>771071</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1927678</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113392</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{430156CA-B71A-FE4A-889D-A2C814B05BDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14487071" y="5091793"/>
+          <a:ext cx="3315607" cy="177799"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1065893</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1916339</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>113392</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E917C0BC-B8E3-DE48-A249-032DB8BF3FAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14781893" y="5269593"/>
+          <a:ext cx="3009446" cy="177799"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>907143</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1909989</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23362F17-B2AF-BA41-810F-BA1776C3C8E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14623143" y="5452382"/>
+          <a:ext cx="3161846" cy="2094593"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>827768</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D946334D-9FCE-3346-A0CA-F47729FC5A3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14543768" y="2780393"/>
+          <a:ext cx="3281589" cy="3223078"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>669018</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4355C9-1DC7-F748-8FF7-95D1CBF34E6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8111218" y="4024993"/>
+          <a:ext cx="9654671" cy="5432274"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>669018</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1872074</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>75259</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A28AA3AE-7F3D-D64F-AA57-36E1AEAE0C6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8111218" y="4202793"/>
+          <a:ext cx="9635856" cy="5245066"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>680357</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2092960</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>102054</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CD602E1-F10E-944C-8D12-5A6ABD5A573E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6154057" y="3291840"/>
+          <a:ext cx="5540103" cy="544014"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>793750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1893660</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>124732</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7D6065A-CF77-7049-97E9-302E8BD64927}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14509750" y="3313793"/>
+          <a:ext cx="3258910" cy="2856139"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1574800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B4D7A49-DD5B-0543-9800-C42EF1BA4166}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7048500" y="6314440"/>
+          <a:ext cx="4655820" cy="3713480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -4209,6 +5467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B44A927-A882-3743-B3D8-A9052DE973A6}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:M60"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" workbookViewId="0"/>
@@ -4821,6 +6080,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D4ED49-275E-7E4A-BA8A-0F7580125B37}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:N90"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" workbookViewId="0"/>
@@ -5624,9 +6884,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624FF2EF-F1A6-254C-9967-68AF7C1C66F8}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:N90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5635,7 +6898,8 @@
     <col min="3" max="3" width="32.3984375" customWidth="1"/>
     <col min="4" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="8" max="10" width="31" customWidth="1"/>
+    <col min="8" max="8" width="33.796875" customWidth="1"/>
+    <col min="9" max="10" width="31" customWidth="1"/>
     <col min="11" max="11" width="3" customWidth="1"/>
     <col min="12" max="13" width="31" customWidth="1"/>
     <col min="14" max="14" width="3" customWidth="1"/>
@@ -6049,6 +7313,12 @@
       <c r="D34" t="s">
         <v>102</v>
       </c>
+      <c r="H34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I34" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
@@ -6152,6 +7422,12 @@
       <c r="D42" t="s">
         <v>116</v>
       </c>
+      <c r="H42" t="s">
+        <v>135</v>
+      </c>
+      <c r="I42" t="s">
+        <v>136</v>
+      </c>
       <c r="L42" s="6"/>
       <c r="M42" s="3"/>
     </row>
@@ -6170,6 +7446,12 @@
       </c>
       <c r="F43" t="s">
         <v>85</v>
+      </c>
+      <c r="H43" t="s">
+        <v>138</v>
+      </c>
+      <c r="I43" t="s">
+        <v>137</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>86</v>
@@ -6307,6 +7589,9 @@
       <c r="M53" s="2"/>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>139</v>
+      </c>
       <c r="L54" t="s">
         <v>35</v>
       </c>
@@ -6314,39 +7599,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" t="s">
-        <v>90</v>
-      </c>
-      <c r="D55" t="s">
-        <v>91</v>
-      </c>
-    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="56" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="57" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="59" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C59" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D59" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>20</v>
@@ -6355,42 +7630,52 @@
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="61" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C61" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C62" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="63" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C63" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C64" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C66" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C67" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2"/>
     <row r="70" spans="3:3" x14ac:dyDescent="0.2"/>
     <row r="71" spans="3:3" x14ac:dyDescent="0.2"/>
     <row r="72" spans="3:3" x14ac:dyDescent="0.2"/>
@@ -6423,4 +7708,832 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A0F2C8-AA8B-7D4A-A8A6-6626E9162631}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="B1:N90"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.3984375" customWidth="1"/>
+    <col min="4" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="8" max="8" width="33.796875" customWidth="1"/>
+    <col min="9" max="10" width="31" customWidth="1"/>
+    <col min="11" max="11" width="3" customWidth="1"/>
+    <col min="12" max="13" width="31" customWidth="1"/>
+    <col min="14" max="14" width="3" customWidth="1"/>
+    <col min="15" max="16384" width="11" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:14" ht="26" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="L15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" t="s">
+        <v>94</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" t="s">
+        <v>41</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" t="s">
+        <v>143</v>
+      </c>
+      <c r="I34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J41" t="s">
+        <v>63</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="2:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" t="s">
+        <v>116</v>
+      </c>
+      <c r="H42" t="s">
+        <v>135</v>
+      </c>
+      <c r="I42" t="s">
+        <v>136</v>
+      </c>
+      <c r="L42" s="6"/>
+      <c r="M42" s="3"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43" t="s">
+        <v>138</v>
+      </c>
+      <c r="I43" t="s">
+        <v>137</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" t="s">
+        <v>127</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" t="s">
+        <v>83</v>
+      </c>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L46" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" t="s">
+        <v>70</v>
+      </c>
+      <c r="L47" t="s">
+        <v>92</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
+        <v>93</v>
+      </c>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" t="s">
+        <v>76</v>
+      </c>
+      <c r="F52" t="s">
+        <v>85</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" t="s">
+        <v>76</v>
+      </c>
+      <c r="F53" t="s">
+        <v>85</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>141</v>
+      </c>
+      <c r="L54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" t="s">
+        <v>118</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C64" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="81" x14ac:dyDescent="0.2"/>
+    <row r="82" x14ac:dyDescent="0.2"/>
+    <row r="83" x14ac:dyDescent="0.2"/>
+    <row r="84" x14ac:dyDescent="0.2"/>
+    <row r="85" x14ac:dyDescent="0.2"/>
+    <row r="86" x14ac:dyDescent="0.2"/>
+    <row r="87" x14ac:dyDescent="0.2"/>
+    <row r="88" x14ac:dyDescent="0.2"/>
+    <row r="89" x14ac:dyDescent="0.2"/>
+    <row r="90" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="L41:M41"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
OO Tic Tac Toe Bonus - AI refinements and choose player markers
</commit_message>
<xml_diff>
--- a/lesson_5/Tic_Tac_Toe_CRC.xlsx
+++ b/lesson_5/Tic_Tac_Toe_CRC.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CB30E3-FB2B-A34B-A0A1-5DE189E7DF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9979D60-D243-8C40-B08D-A6B03304DE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
+    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="4" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Game" sheetId="1" r:id="rId1"/>
     <sheet name="Scored Game" sheetId="2" r:id="rId2"/>
     <sheet name="AI Defense" sheetId="3" r:id="rId3"/>
     <sheet name="AI Offense" sheetId="4" r:id="rId4"/>
+    <sheet name="AI Refinement" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="147">
   <si>
     <t>Board</t>
   </si>
@@ -451,6 +452,9 @@
     <t>two_taken_one_empty?</t>
   </si>
   <si>
+    <t>Can determine if square is empty</t>
+  </si>
+  <si>
     <t>empty_square</t>
   </si>
   <si>
@@ -470,6 +474,12 @@
   </si>
   <si>
     <t>Can determine if one empty in line</t>
+  </si>
+  <si>
+    <t>empty?</t>
+  </si>
+  <si>
+    <t>Board.empty?</t>
   </si>
 </sst>
 </file>
@@ -5142,6 +5152,1230 @@
         <a:xfrm flipH="1">
           <a:off x="7048500" y="6314440"/>
           <a:ext cx="4655820" cy="3713480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>918482</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>170089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B73CFB-F406-C740-BEA8-6CD6DA30A08B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8360682" y="7282089"/>
+          <a:ext cx="9405207" cy="1501608"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>918482</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1900296</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>102053</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C540535E-DE65-0646-BA6C-0C1BD4D33AE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8360682" y="8783697"/>
+          <a:ext cx="9414614" cy="868756"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>903111</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>103481</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234C15D6-F12A-1541-A1A8-5C9C22BC7C1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8345311" y="8783697"/>
+          <a:ext cx="9420578" cy="1047984"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>799630</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>159926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1900296</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>112889</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97567B90-976C-A044-B73E-E8C683439994}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8241830" y="8110126"/>
+          <a:ext cx="9533466" cy="664163"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>703036</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2113280</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEEFB3FC-72F3-3B44-A947-63389458989E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6176736" y="5267960"/>
+          <a:ext cx="5537744" cy="1980112"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>855436</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2082800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>107044</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D51A8D7-5E08-FB4C-8C09-5B1AAB3E4F18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6329136" y="5791200"/>
+          <a:ext cx="5354864" cy="1605644"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1564822</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2113280</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09E033C7-435D-A44A-A2C6-DDA510E9D0FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7038522" y="5633720"/>
+          <a:ext cx="4675958" cy="1833880"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>884465</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2092960</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>147411</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E75861CB-6515-A442-9D33-844F5B20232C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6358165" y="5476240"/>
+          <a:ext cx="5335995" cy="4043771"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1678215</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2092960</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>22678</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FE4EDD8-7586-A142-9492-AFC27D0D83FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7151915" y="5069840"/>
+          <a:ext cx="4542245" cy="4503238"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1185333</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F6C2026-11A7-0049-9E45-C24FFA10D847}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6659033" y="5455920"/>
+          <a:ext cx="5045287" cy="4356946"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1749778</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2092960</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>65852</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70E2112A-4BED-E444-AB98-6B944B8446A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7223478" y="5080000"/>
+          <a:ext cx="4470682" cy="4714052"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1345259</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2072640</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>122296</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFF8B750-0B0F-574B-97C0-3CB40AD290A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6818959" y="5999480"/>
+          <a:ext cx="4854881" cy="2073016"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>743185</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94074</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{647BC096-1F57-834A-A0C7-1C73F68FB75F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6216885" y="6156960"/>
+          <a:ext cx="5487435" cy="2242914"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>771071</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1927678</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113392</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA2F9E94-C0A6-5F40-905D-1680453CEB46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14487071" y="5091793"/>
+          <a:ext cx="3315607" cy="177799"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1065893</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1916339</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>113392</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A808A0-7C49-034C-BC83-2D2F20603411}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14781893" y="5269593"/>
+          <a:ext cx="3009446" cy="177799"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>907143</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1909989</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF10F62-850A-DF42-AE92-4B1A5CEE02AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14623143" y="5452382"/>
+          <a:ext cx="3161846" cy="2094593"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>827768</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1950357</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A272433-AEB7-3440-82A4-6360890700AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14543768" y="2780393"/>
+          <a:ext cx="3281589" cy="3223078"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>669018</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1890889</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF58EF75-B720-0347-9779-8620C8CEC098}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8111218" y="4024993"/>
+          <a:ext cx="9654671" cy="5432274"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>669018</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1872074</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>75259</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8978D571-C8A3-724D-8F1B-20A45720C7E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8111218" y="4202793"/>
+          <a:ext cx="9635856" cy="5245066"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>680357</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2092960</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>102054</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FB50354-B181-304E-B28B-BDAA9B3CE9C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6154057" y="3291840"/>
+          <a:ext cx="5540103" cy="544014"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>793750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1893660</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>124732</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04744B0E-5029-894C-B7FF-22C610268B7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14509750" y="3313793"/>
+          <a:ext cx="3258910" cy="2856139"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1574800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F2F7132-4EB8-B047-9DA0-81E01E2529C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7048500" y="6314440"/>
+          <a:ext cx="4655820" cy="3713480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1564640</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F7F0D58-6C91-6D47-813E-31E145E57E17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7038340" y="6492240"/>
+          <a:ext cx="4665980" cy="3723640"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6887,9 +8121,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:N90"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7448,10 +8680,10 @@
         <v>85</v>
       </c>
       <c r="H43" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" t="s">
         <v>138</v>
-      </c>
-      <c r="I43" t="s">
-        <v>137</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>86</v>
@@ -7590,7 +8822,7 @@
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.2">
       <c r="E54" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L54" t="s">
         <v>35</v>
@@ -7715,8 +8947,834 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:N90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.3984375" customWidth="1"/>
+    <col min="4" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="8" max="8" width="33.796875" customWidth="1"/>
+    <col min="9" max="10" width="31" customWidth="1"/>
+    <col min="11" max="11" width="3" customWidth="1"/>
+    <col min="12" max="13" width="31" customWidth="1"/>
+    <col min="14" max="14" width="3" customWidth="1"/>
+    <col min="15" max="16384" width="11" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:14" ht="26" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="L15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" t="s">
+        <v>94</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" t="s">
+        <v>41</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" t="s">
+        <v>144</v>
+      </c>
+      <c r="I34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J41" t="s">
+        <v>63</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="2:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" t="s">
+        <v>116</v>
+      </c>
+      <c r="H42" t="s">
+        <v>135</v>
+      </c>
+      <c r="I42" t="s">
+        <v>136</v>
+      </c>
+      <c r="L42" s="6"/>
+      <c r="M42" s="3"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" t="s">
+        <v>138</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" t="s">
+        <v>127</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" t="s">
+        <v>83</v>
+      </c>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L46" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" t="s">
+        <v>70</v>
+      </c>
+      <c r="L47" t="s">
+        <v>92</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
+        <v>93</v>
+      </c>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" t="s">
+        <v>76</v>
+      </c>
+      <c r="F52" t="s">
+        <v>85</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" t="s">
+        <v>76</v>
+      </c>
+      <c r="F53" t="s">
+        <v>85</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>142</v>
+      </c>
+      <c r="L54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" t="s">
+        <v>118</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C64" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2"/>
+    <row r="81" x14ac:dyDescent="0.2"/>
+    <row r="82" x14ac:dyDescent="0.2"/>
+    <row r="83" x14ac:dyDescent="0.2"/>
+    <row r="84" x14ac:dyDescent="0.2"/>
+    <row r="85" x14ac:dyDescent="0.2"/>
+    <row r="86" x14ac:dyDescent="0.2"/>
+    <row r="87" x14ac:dyDescent="0.2"/>
+    <row r="88" x14ac:dyDescent="0.2"/>
+    <row r="89" x14ac:dyDescent="0.2"/>
+    <row r="90" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="L41:M41"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E787865A-2D53-2E40-B8D7-C6AC60E2FBBF}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="B1:N90"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -7737,7 +9795,7 @@
     <row r="1" spans="2:14" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:14" ht="26" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2"/>
@@ -8142,10 +10200,10 @@
         <v>102</v>
       </c>
       <c r="H34" t="s">
+        <v>144</v>
+      </c>
+      <c r="I34" t="s">
         <v>143</v>
-      </c>
-      <c r="I34" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.2">
@@ -8157,6 +10215,12 @@
       </c>
       <c r="D35" t="s">
         <v>130</v>
+      </c>
+      <c r="H35" t="s">
+        <v>137</v>
+      </c>
+      <c r="I35" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
@@ -8276,10 +10340,10 @@
         <v>85</v>
       </c>
       <c r="H43" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" t="s">
         <v>138</v>
-      </c>
-      <c r="I43" t="s">
-        <v>137</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>86</v>
@@ -8418,7 +10482,7 @@
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.2">
       <c r="E54" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L54" t="s">
         <v>35</v>
@@ -8427,7 +10491,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>146</v>
+      </c>
+    </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.2"/>
     <row r="57" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B57" t="s">

</xml_diff>